<commit_message>
update trước khi về tết
</commit_message>
<xml_diff>
--- a/TDStore/ABac2.xlsx
+++ b/TDStore/ABac2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10.NewPC\01.TDStore\04.Private\TDStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8230664-6FB3-49A6-B066-7B6364863C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4C474-D325-4DDC-BFE6-6AB4E4F3EDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11.12.23" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,27 @@
     <sheet name="6.1.24" sheetId="3" r:id="rId3"/>
     <sheet name="28.1.24" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
   <si>
     <t>Tên</t>
   </si>
@@ -118,6 +128,15 @@
   </si>
   <si>
     <t>Đã xong</t>
+  </si>
+  <si>
+    <t>Chuyển ngày 5.2.24</t>
+  </si>
+  <si>
+    <t>Chuyển sang công nợ ngày 6.1.24</t>
+  </si>
+  <si>
+    <t>Đã trả ngày 5.2.24</t>
   </si>
 </sst>
 </file>
@@ -269,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -309,6 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,10 +338,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,15 +624,15 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -630,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>7490</v>
       </c>
@@ -645,7 +661,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -660,7 +676,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>9305</v>
       </c>
@@ -675,7 +691,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -690,7 +706,7 @@
         <v>18500000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -705,7 +721,7 @@
         <v>5800000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -720,7 +736,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -735,7 +751,7 @@
         <v>6200000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -750,7 +766,7 @@
         <v>6700000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D11" s="10">
         <f>SUM(D2:D9)</f>
         <v>66200000</v>
@@ -759,7 +775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -773,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -788,7 +804,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D16" s="11">
         <f>SUM(D14:D14)</f>
         <v>200000</v>
@@ -797,19 +813,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="D19" s="13">
         <f>D11-D16</f>
         <v>66000000</v>
       </c>
       <c r="E19" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="31" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D21" s="27" t="s">
         <v>29</v>
       </c>
     </row>
@@ -824,21 +840,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518E3E15-0D78-4F6C-B4C7-E01F0536B4E1}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -853,7 +869,7 @@
       </c>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -869,7 +885,7 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -885,7 +901,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -901,7 +917,7 @@
       </c>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>16</v>
       </c>
@@ -917,7 +933,7 @@
       </c>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>17</v>
       </c>
@@ -933,7 +949,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>18</v>
       </c>
@@ -949,7 +965,7 @@
       </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
@@ -965,7 +981,7 @@
       </c>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -981,7 +997,7 @@
       </c>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -997,7 +1013,7 @@
       </c>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="19"/>
       <c r="D11" s="10">
         <f>SUM(D2:D10)</f>
@@ -1007,11 +1023,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1042,7 @@
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>22</v>
       </c>
@@ -1042,7 +1058,7 @@
       </c>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>23</v>
       </c>
@@ -1058,7 +1074,7 @@
       </c>
       <c r="E15" s="20"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>26</v>
       </c>
@@ -1074,39 +1090,56 @@
       </c>
       <c r="E16" s="20"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="8">
+        <v>70000000</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <f>B17*C17</f>
+        <v>70000000</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
       <c r="D18" s="11">
-        <f>SUM(D14:D16)</f>
-        <v>52150000</v>
+        <f>SUM(D14:D17)</f>
+        <v>122150000</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
       <c r="E19" s="20"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="24"/>
       <c r="D21" s="25">
         <f>D11-D18</f>
-        <v>63250000</v>
-      </c>
-      <c r="E21" s="26"/>
+        <v>-6750000</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1121,19 +1154,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BCEF21-9D1E-48DB-9392-20A8F9275E7E}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1181,7 @@
       </c>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1197,7 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1213,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
@@ -1196,7 +1229,7 @@
       </c>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1245,7 @@
       </c>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
@@ -1228,11 +1261,10 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D8" s="10">
         <f>SUM(D2:D6)</f>
         <v>72950000</v>
@@ -1241,11 +1273,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="19"/>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
@@ -1260,7 +1292,7 @@
       </c>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>24</v>
       </c>
@@ -1276,7 +1308,7 @@
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>22</v>
       </c>
@@ -1287,12 +1319,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" ref="D12:D13" si="1">B12*C12</f>
+        <f t="shared" ref="D12:D14" si="1">B12*C12</f>
         <v>500000</v>
       </c>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>28</v>
       </c>
@@ -1308,37 +1340,49 @@
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8">
+        <v>6750000</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
+        <v>6750000</v>
+      </c>
       <c r="E14" s="20"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="19"/>
       <c r="D15" s="11">
-        <f>SUM(D11:D12)</f>
-        <v>1000000</v>
+        <f>SUM(D11:D14)</f>
+        <v>7950000</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="19"/>
       <c r="E16" s="20"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="24"/>
       <c r="D18" s="25">
         <f>D8-D15</f>
-        <v>71950000</v>
+        <v>65000000</v>
       </c>
       <c r="E18" s="26"/>
     </row>
@@ -1359,15 +1403,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1426,7 @@
       </c>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1442,7 @@
       </c>
       <c r="E2" s="20"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>17</v>
       </c>
@@ -1414,7 +1458,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
@@ -1430,7 +1474,7 @@
       </c>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="19"/>
       <c r="D5" s="10">
         <f>SUM(D2:D4)</f>
@@ -1440,11 +1484,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="22" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1503,7 @@
       </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1519,7 @@
       </c>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
@@ -1491,7 +1535,7 @@
       </c>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
@@ -1507,7 +1551,7 @@
       </c>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="19"/>
       <c r="D11" s="11">
         <f>SUM(D8:D9)</f>
@@ -1517,19 +1561,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="19"/>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="24"/>
       <c r="D14" s="25">
         <f>D5-D11</f>

</xml_diff>

<commit_message>
Update sau ban cho anh Bac 10 may 7400, anh thanh 9420
</commit_message>
<xml_diff>
--- a/TDStore/ABac2.xlsx
+++ b/TDStore/ABac2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\TDStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10.NewPC\01.TDStore\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C58865B-4227-4712-8AF6-86A407E49C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E620B34-4E78-4AAA-BFEF-1358E4C1AC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11.12.23" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="6.1.24" sheetId="3" r:id="rId3"/>
     <sheet name="28.1.24" sheetId="4" r:id="rId4"/>
     <sheet name="20.2.24" sheetId="5" r:id="rId5"/>
+    <sheet name="17.3.24" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
   <si>
     <t>Tên</t>
   </si>
@@ -152,6 +153,21 @@
   </si>
   <si>
     <t>Đã trả ngày 23.2.24</t>
+  </si>
+  <si>
+    <t>Ngày 17.3.24</t>
+  </si>
+  <si>
+    <t>7400B i5/16/256</t>
+  </si>
+  <si>
+    <t>Đã trả ngày 9.3.24</t>
+  </si>
+  <si>
+    <t>Chuyển sang công nợ ngày 28.1</t>
+  </si>
+  <si>
+    <t>Chuyển công nợ ngày 6.1</t>
   </si>
 </sst>
 </file>
@@ -639,15 +655,15 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -661,7 +677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>7490</v>
       </c>
@@ -676,7 +692,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -691,7 +707,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>9305</v>
       </c>
@@ -706,7 +722,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -721,7 +737,7 @@
         <v>18500000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -736,7 +752,7 @@
         <v>5800000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -751,7 +767,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -766,7 +782,7 @@
         <v>6200000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -781,7 +797,7 @@
         <v>6700000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" s="10">
         <f>SUM(D2:D9)</f>
         <v>66200000</v>
@@ -790,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -804,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -819,7 +835,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="11">
         <f>SUM(D14:D14)</f>
         <v>200000</v>
@@ -828,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>5</v>
       </c>
@@ -839,7 +855,7 @@
       </c>
       <c r="E19" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="26" t="s">
         <v>29</v>
       </c>
@@ -861,16 +877,16 @@
       <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -887,7 +903,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
@@ -903,7 +919,7 @@
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
@@ -919,7 +935,7 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>15</v>
       </c>
@@ -935,7 +951,7 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>16</v>
       </c>
@@ -951,7 +967,7 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
@@ -967,7 +983,7 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>18</v>
       </c>
@@ -983,7 +999,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>19</v>
       </c>
@@ -999,7 +1015,7 @@
       </c>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
@@ -1015,7 +1031,7 @@
       </c>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
@@ -1031,7 +1047,7 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="D11" s="10">
         <f>SUM(D2:D10)</f>
@@ -1041,11 +1057,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1076,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>22</v>
       </c>
@@ -1076,7 +1092,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
@@ -1092,7 +1108,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1124,7 @@
       </c>
       <c r="E16" s="19"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>26</v>
       </c>
@@ -1126,7 +1142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="D18" s="11">
         <f>SUM(D14:D17)</f>
@@ -1136,15 +1152,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>5</v>
       </c>
@@ -1170,22 +1186,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BCEF21-9D1E-48DB-9392-20A8F9275E7E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -1218,7 +1234,7 @@
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -1234,7 +1250,7 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1266,7 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
@@ -1266,7 +1282,7 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -1282,10 +1298,10 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" s="10">
         <f>SUM(D2:D6)</f>
         <v>72950000</v>
@@ -1294,11 +1310,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>4</v>
       </c>
@@ -1313,7 +1329,7 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1345,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>22</v>
       </c>
@@ -1340,12 +1356,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" ref="D12:D15" si="1">B12*C12</f>
+        <f t="shared" ref="D12:D16" si="1">B12*C12</f>
         <v>500000</v>
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>28</v>
       </c>
@@ -1361,7 +1377,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>32</v>
       </c>
@@ -1377,7 +1393,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>40</v>
       </c>
@@ -1393,39 +1409,57 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="18"/>
-      <c r="D16" s="11">
-        <f>SUM(D11:D15)</f>
-        <v>57950000</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8">
+        <v>30000000</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="1"/>
+        <v>30000000</v>
+      </c>
+      <c r="E16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D17" s="11">
+        <f>SUM(D11:D16)</f>
+        <v>87950000</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24">
-        <f>D8-D16</f>
-        <v>15000000</v>
-      </c>
-      <c r="E19" s="25"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24">
+        <f>D8-D17</f>
+        <v>-15000000</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1434,22 +1468,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F92984B-B13F-4671-BC36-F2DAB26D9586}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +1500,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
@@ -1482,7 +1516,7 @@
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>17</v>
       </c>
@@ -1498,7 +1532,7 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
@@ -1514,7 +1548,7 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="D5" s="10">
         <f>SUM(D2:D4)</f>
@@ -1524,11 +1558,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1577,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
@@ -1559,7 +1593,7 @@
       </c>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
@@ -1570,12 +1604,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" ref="D9:D10" si="1">C9*B9</f>
+        <f t="shared" ref="D9:D11" si="1">C9*B9</f>
         <v>250000</v>
       </c>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>28</v>
       </c>
@@ -1591,39 +1625,59 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="18"/>
-      <c r="D11" s="11">
-        <f>SUM(D8:D9)</f>
-        <v>550000</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="8">
+        <v>15000000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="1"/>
+        <v>15000000</v>
+      </c>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="29" t="s">
+      <c r="D13" s="11">
+        <f>SUM(D8:D11)</f>
+        <v>15750000</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24">
-        <f>D5-D11</f>
-        <v>54050000</v>
-      </c>
-      <c r="E14" s="25"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24">
+        <f>D5-D13</f>
+        <v>38850000</v>
+      </c>
+      <c r="E16" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1634,20 +1688,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABE387F-77DA-466B-85F9-C8A9BC91CF5C}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.1328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1664,7 +1718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>33</v>
       </c>
@@ -1680,7 +1734,7 @@
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>38</v>
       </c>
@@ -1696,7 +1750,7 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>39</v>
       </c>
@@ -1712,7 +1766,7 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="D5" s="10">
         <f>SUM(D2:D4)</f>
@@ -1722,11 +1776,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
@@ -1741,19 +1795,19 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="E8" s="19"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="D11" s="11">
         <f>SUM(D8:D9)</f>
@@ -1763,15 +1817,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>5</v>
       </c>
@@ -1780,6 +1834,144 @@
       <c r="D14" s="24">
         <f>D5-D11</f>
         <v>42000000</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B988ED-FC2F-47D6-AD32-A8BAFCBA608F}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5800000</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D4" si="0">B2*C2</f>
+        <v>58000000</v>
+      </c>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="D5" s="10">
+        <f>SUM(D2:D4)</f>
+        <v>58000000</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="D11" s="11">
+        <f>SUM(D8:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24">
+        <f>D5-D11</f>
+        <v>58000000</v>
       </c>
       <c r="E14" s="25"/>
     </row>

</xml_diff>

<commit_message>
Update công nợ + phí ship
</commit_message>
<xml_diff>
--- a/TDStore/ABac2.xlsx
+++ b/TDStore/ABac2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10.NewPC\01.TDStore\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B24D9E7-23EA-43B2-B3EA-98FBE7132D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C0D41B-EFDD-404D-8EF0-13D14CF440F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2985" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11.12.23" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
   <si>
     <t>Tên</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>Ngày 20.3.24</t>
+  </si>
+  <si>
+    <t>Chuyển khoản ngày 23.3.24</t>
+  </si>
+  <si>
+    <t>Chuyển sang ngày 17.3</t>
+  </si>
+  <si>
+    <t>Chuyển công nợ ngày 20.2.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin </t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1505,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F16"/>
+      <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABE387F-77DA-466B-85F9-C8A9BC91CF5C}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1746,7 @@
     <col min="2" max="2" width="14.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,7 +1860,19 @@
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="8">
+        <v>50000000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <f>C9*B9</f>
+        <v>50000000</v>
+      </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1859,7 +1883,7 @@
       <c r="A11" s="18"/>
       <c r="D11" s="11">
         <f>SUM(D8:D9)</f>
-        <v>41150000</v>
+        <v>91150000</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>3</v>
@@ -1881,9 +1905,11 @@
       <c r="C14" s="23"/>
       <c r="D14" s="24">
         <f>D5-D11</f>
-        <v>850000</v>
-      </c>
-      <c r="E14" s="25"/>
+        <v>-49150000</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2001,17 +2027,39 @@
       <c r="A9" s="18" t="s">
         <v>50</v>
       </c>
+      <c r="B9" s="8">
+        <v>400000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <f>C9*B9</f>
+        <v>400000</v>
+      </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="8">
+        <v>49150000</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <f>C10*B10</f>
+        <v>49150000</v>
+      </c>
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="D11" s="11">
-        <f>SUM(D8:D9)</f>
-        <v>500000</v>
+        <f>SUM(D8:D10)</f>
+        <v>50050000</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>3</v>
@@ -2033,7 +2081,7 @@
       <c r="C14" s="23"/>
       <c r="D14" s="24">
         <f>D5-D11</f>
-        <v>57500000</v>
+        <v>7950000</v>
       </c>
       <c r="E14" s="25"/>
     </row>
@@ -2050,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514BB4DB-55F3-4BAD-AFB8-182315A864EC}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,11 +2182,35 @@
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8">
+        <v>200000</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <f>C8*B8</f>
+        <v>200000</v>
+      </c>
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="8">
+        <v>250000</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <f>C9*B9</f>
+        <v>500000</v>
+      </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2149,7 +2221,7 @@
       <c r="A11" s="18"/>
       <c r="D11" s="11">
         <f>SUM(D8:D9)</f>
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>3</v>
@@ -2171,7 +2243,7 @@
       <c r="C14" s="23"/>
       <c r="D14" s="24">
         <f>D5-D11</f>
-        <v>79200000</v>
+        <v>78500000</v>
       </c>
       <c r="E14" s="25"/>
     </row>

</xml_diff>